<commit_message>
Updates Template minutiae types
Minutiae types are now correct. Both files still have 1 incorrect data
each, which are marked in yellow.
</commit_message>
<xml_diff>
--- a/TestData/Perfect minutiae/Normal fingers/T_Ale1439794734-Hamster-1-1.xlsx
+++ b/TestData/Perfect minutiae/Normal fingers/T_Ale1439794734-Hamster-1-1.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Final Template" sheetId="3" r:id="rId2"/>
     <sheet name="Support Data" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -168,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -206,6 +206,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,7 +558,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C2">
@@ -611,8 +612,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>15</v>
+      <c r="B3" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="C3">
         <v>115.91800000000001</v>
@@ -629,7 +630,7 @@
       </c>
       <c r="I3" t="str">
         <f>IF(B3='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J36" si="1">DEC2HEX(C3, 2)</f>
@@ -645,7 +646,7 @@
       </c>
       <c r="M3" t="str">
         <f>CONCATENATE(I3,J3,'Support Data'!$C$7,K3,L3,'Support Data'!$C$8)</f>
-        <v>8073003CFA00</v>
+        <v>4073003CFA00</v>
       </c>
       <c r="P3" s="13"/>
       <c r="Q3" s="14"/>
@@ -659,8 +660,8 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>16</v>
+      <c r="B4" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C4">
         <v>182.857</v>
@@ -677,7 +678,7 @@
       </c>
       <c r="I4" t="str">
         <f>IF(B4='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="1"/>
@@ -706,8 +707,8 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>16</v>
+      <c r="B5" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C5">
         <v>49.387999999999998</v>
@@ -724,7 +725,7 @@
       </c>
       <c r="I5" t="str">
         <f>IF(B5='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="1"/>
@@ -740,7 +741,7 @@
       </c>
       <c r="M5" t="str">
         <f>CONCATENATE(I5,J5,'Support Data'!$C$7,K5,L5,'Support Data'!$C$8)</f>
-        <v>4031005E9400</v>
+        <v>8031005E9400</v>
       </c>
       <c r="Q5" s="14"/>
       <c r="R5" s="14"/>
@@ -753,7 +754,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C6">
@@ -794,7 +795,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C7">
@@ -835,7 +836,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C8">
@@ -876,7 +877,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C9">
@@ -916,11 +917,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C10">
@@ -965,7 +966,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C11">
@@ -1006,7 +1007,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C12">
@@ -1047,8 +1048,8 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>15</v>
+      <c r="B13" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="C13">
         <v>161.63300000000001</v>
@@ -1065,7 +1066,7 @@
       </c>
       <c r="I13" t="str">
         <f>IF(B13='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="1"/>
@@ -1081,15 +1082,15 @@
       </c>
       <c r="M13" t="str">
         <f>CONCATENATE(I13,J13,'Support Data'!$C$7,K13,L13,'Support Data'!$C$8)</f>
-        <v>80A100ACF200</v>
+        <v>40A100ACF200</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>15</v>
+      <c r="B14" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="C14">
         <v>181.63300000000001</v>
@@ -1106,7 +1107,7 @@
       </c>
       <c r="I14" t="str">
         <f>IF(B14='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="1"/>
@@ -1122,14 +1123,14 @@
       </c>
       <c r="M14" t="str">
         <f>CONCATENATE(I14,J14,'Support Data'!$C$7,K14,L14,'Support Data'!$C$8)</f>
-        <v>80B500B47100</v>
+        <v>40B500B47100</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C15">
@@ -1170,7 +1171,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -1211,8 +1212,8 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>16</v>
+      <c r="B17" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C17">
         <v>220.816</v>
@@ -1229,7 +1230,7 @@
       </c>
       <c r="I17" t="str">
         <f>IF(B17='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="1"/>
@@ -1245,15 +1246,15 @@
       </c>
       <c r="M17" t="str">
         <f>CONCATENATE(I17,J17,'Support Data'!$C$7,K17,L17,'Support Data'!$C$8)</f>
-        <v>40DC00E96900</v>
+        <v>80DC00E96900</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>16</v>
+      <c r="B18" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C18">
         <v>171.429</v>
@@ -1270,7 +1271,7 @@
       </c>
       <c r="I18" t="str">
         <f>IF(B18='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="1"/>
@@ -1286,15 +1287,15 @@
       </c>
       <c r="M18" t="str">
         <f>CONCATENATE(I18,J18,'Support Data'!$C$7,K18,L18,'Support Data'!$C$8)</f>
-        <v>40AB00DF7000</v>
+        <v>80AB00DF7000</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>15</v>
+      <c r="B19" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="C19">
         <v>144.898</v>
@@ -1311,7 +1312,7 @@
       </c>
       <c r="I19" t="str">
         <f>IF(B19='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="1"/>
@@ -1327,14 +1328,14 @@
       </c>
       <c r="M19" t="str">
         <f>CONCATENATE(I19,J19,'Support Data'!$C$7,K19,L19,'Support Data'!$C$8)</f>
-        <v>809000E6F200</v>
+        <v>409000E6F200</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C20">
@@ -1375,7 +1376,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C21">
@@ -1416,7 +1417,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C22">
@@ -1457,7 +1458,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C23">
@@ -1498,8 +1499,8 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>15</v>
+      <c r="B24" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="C24">
         <v>140</v>
@@ -1516,7 +1517,7 @@
       </c>
       <c r="I24" t="str">
         <f>IF(B24='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="1"/>
@@ -1532,14 +1533,14 @@
       </c>
       <c r="M24" t="str">
         <f>CONCATENATE(I24,J24,'Support Data'!$C$7,K24,L24,'Support Data'!$C$8)</f>
-        <v>808C00ED8000</v>
+        <v>408C00ED8000</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C25">
@@ -1580,8 +1581,8 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>16</v>
+      <c r="B26" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C26">
         <v>197.959</v>
@@ -1598,7 +1599,7 @@
       </c>
       <c r="I26" t="str">
         <f>IF(B26='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="1"/>
@@ -1614,14 +1615,14 @@
       </c>
       <c r="M26" t="str">
         <f>CONCATENATE(I26,J26,'Support Data'!$C$7,K26,L26,'Support Data'!$C$8)</f>
-        <v>40C5010DDB00</v>
+        <v>80C5010DDB00</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C27">
@@ -1662,8 +1663,8 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>15</v>
+      <c r="B28" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="C28">
         <v>155.91800000000001</v>
@@ -1680,7 +1681,7 @@
       </c>
       <c r="I28" t="str">
         <f>IF(B28='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="1"/>
@@ -1696,15 +1697,15 @@
       </c>
       <c r="M28" t="str">
         <f>CONCATENATE(I28,J28,'Support Data'!$C$7,K28,L28,'Support Data'!$C$8)</f>
-        <v>809B010F6700</v>
+        <v>409B010F6700</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>16</v>
+      <c r="B29" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C29">
         <v>47.755000000000003</v>
@@ -1721,7 +1722,7 @@
       </c>
       <c r="I29" t="str">
         <f>IF(B29='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="1"/>
@@ -1737,14 +1738,14 @@
       </c>
       <c r="M29" t="str">
         <f>CONCATENATE(I29,J29,'Support Data'!$C$7,K29,L29,'Support Data'!$C$8)</f>
-        <v>402F01372800</v>
+        <v>802F01372800</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C30">
@@ -1785,7 +1786,7 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C31">
@@ -1826,8 +1827,8 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>15</v>
+      <c r="B32" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="C32">
         <v>107.755</v>
@@ -1844,7 +1845,7 @@
       </c>
       <c r="I32" t="str">
         <f>IF(B32='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="1"/>
@@ -1860,14 +1861,14 @@
       </c>
       <c r="M32" t="str">
         <f>CONCATENATE(I32,J32,'Support Data'!$C$7,K32,L32,'Support Data'!$C$8)</f>
-        <v>806B012CF700</v>
+        <v>406B012CF700</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C33">
@@ -1908,8 +1909,8 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>16</v>
+      <c r="B34" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C34">
         <v>247.755</v>
@@ -1926,7 +1927,7 @@
       </c>
       <c r="I34" t="str">
         <f>IF(B34='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="1"/>
@@ -1942,14 +1943,14 @@
       </c>
       <c r="M34" t="str">
         <f>CONCATENATE(I34,J34,'Support Data'!$C$7,K34,L34,'Support Data'!$C$8)</f>
-        <v>40F701106200</v>
+        <v>80F701106200</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C35">
@@ -1990,8 +1991,8 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>16</v>
+      <c r="B36" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C36">
         <v>193.87799999999999</v>
@@ -2008,7 +2009,7 @@
       </c>
       <c r="I36" t="str">
         <f>IF(B36='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="1"/>
@@ -2024,7 +2025,7 @@
       </c>
       <c r="M36" t="str">
         <f>CONCATENATE(I36,J36,'Support Data'!$C$7,K36,L36,'Support Data'!$C$8)</f>
-        <v>40C101806800</v>
+        <v>80C101806800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes wrong angle data
Template complete by fixing wrong angle data.
</commit_message>
<xml_diff>
--- a/TestData/Perfect minutiae/Normal fingers/T_Ale1439794734-Hamster-1-1.xlsx
+++ b/TestData/Perfect minutiae/Normal fingers/T_Ale1439794734-Hamster-1-1.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Final Template" sheetId="3" r:id="rId2"/>
     <sheet name="Support Data" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -151,7 +151,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -193,7 +193,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -206,7 +206,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,7 +491,7 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B36"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C2">
@@ -598,9 +598,9 @@
         <f>CONCATENATE('Support Data'!D11,'Support Data'!D12,'Support Data'!D13,'Support Data'!D14)</f>
         <v>464D520020323000000000F00000012C019000C500C5010000105B23</v>
       </c>
-      <c r="Q2" s="14" t="e">
+      <c r="Q2" s="14" t="str">
         <f>CONCATENATE(P2,P10,'Support Data'!C17)</f>
-        <v>#NUM!</v>
+        <v>464D520020323000000000F00000012C019000C500C5010000105B234047002F8F004073003CFA0080B6003D75008031005E94008087005D7E00805D006608004037007795008045008F0600402600A4A000405400A5910040C300A4E60040A100ACF20040B500B47100403900BD1D0040A700CBED0080DC00E9690080AB00DF7000409000E6F200405900DE9300404500E91A00402E0102AD00406600F00F00408C00ED800080B200F8E50080C5010DDB00408400FBF200409B010F6700802F013728004057011B190040A401455C00406B012CF700402B015E280080F70110620040D101736D0080C1018068000000</v>
       </c>
       <c r="R2" s="14"/>
       <c r="S2" s="14"/>
@@ -612,7 +612,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C3">
@@ -660,7 +660,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C4">
@@ -669,12 +669,12 @@
       <c r="D4">
         <v>61.633000000000003</v>
       </c>
-      <c r="E4" s="12">
-        <v>524.93200000000002</v>
+      <c r="E4" s="17">
+        <v>164.93</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>373.28497777777778</v>
+        <v>117.28355555555557</v>
       </c>
       <c r="I4" t="str">
         <f>IF(B4='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
@@ -688,13 +688,13 @@
         <f t="shared" si="2"/>
         <v>003D</v>
       </c>
-      <c r="L4" t="e">
+      <c r="L4" t="str">
         <f>DEC2HEX(F4, 2)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M4" t="e">
+        <v>75</v>
+      </c>
+      <c r="M4" t="str">
         <f>CONCATENATE(I4,J4,'Support Data'!$C$7,K4,L4,'Support Data'!$C$8)</f>
-        <v>#NUM!</v>
+        <v>80B6003D7500</v>
       </c>
       <c r="Q4" s="14"/>
       <c r="R4" s="14"/>
@@ -707,7 +707,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C5">
@@ -754,7 +754,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C6">
@@ -795,7 +795,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C7">
@@ -836,7 +836,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C8">
@@ -877,7 +877,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C9">
@@ -921,7 +921,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C10">
@@ -957,16 +957,16 @@
         <f>CONCATENATE(I10,J10,'Support Data'!$C$7,K10,L10,'Support Data'!$C$8)</f>
         <v>402600A4A000</v>
       </c>
-      <c r="P10" s="1" t="e">
+      <c r="P10" s="1" t="str">
         <f>CONCATENATE(M2,M3,M4,M5,M6,M7,M8,M9,M10,M11,M12,M13,M14,M15,M16,M17,M18,M19,M20,M21,M22,M23,M24,M25,M26,M27,M28,M29,M30,M31,M32,M33,M34,M35,M36,M37,M38,M39,M40,M41,M42,M43,M44,M45,M46,M47,M48,M49,M50,M51,M52,M53,M54,M55,M56,M57,M58,M59,M60,M61,M62,M63,M64,M65,M66,M67,M68,M69,M70,M71,M72,M73,M74,M75,M76,M77,M78,M79,M80,M81,M82,M83,M84,M85,M86,M87,M88,M89,M90,M91,M92,M93,M94,M95,M96,M97,M98,M99,M100,M101,M102,M103,M104,M105,M106,M107,M108,M109,M110,M111,M112,M113,M114,M115,M116,M117,M118,M119,M120,M121,M122,M123,M124,M125,M126,M127,M128,M129,M130,M131,M132,M133,M134,M135,M136,M137,M138,M139,M140,M141,M142,M143,M144,M145,M146,M147,M148,M149,M150)</f>
-        <v>#NUM!</v>
+        <v>4047002F8F004073003CFA0080B6003D75008031005E94008087005D7E00805D006608004037007795008045008F0600402600A4A000405400A5910040C300A4E60040A100ACF20040B500B47100403900BD1D0040A700CBED0080DC00E9690080AB00DF7000409000E6F200405900DE9300404500E91A00402E0102AD00406600F00F00408C00ED800080B200F8E50080C5010DDB00408400FBF200409B010F6700802F013728004057011B190040A401455C00406B012CF700402B015E280080F70110620040D101736D0080C101806800</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C11">
@@ -1007,7 +1007,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C12">
@@ -1048,7 +1048,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C13">
@@ -1089,7 +1089,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C14">
@@ -1130,7 +1130,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C15">
@@ -1171,7 +1171,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -1212,7 +1212,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C17">
@@ -1253,7 +1253,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C18">
@@ -1294,7 +1294,7 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C19">
@@ -1335,7 +1335,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C20">
@@ -1376,7 +1376,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C21">
@@ -1417,7 +1417,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C22">
@@ -1458,7 +1458,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C23">
@@ -1499,7 +1499,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C24">
@@ -1540,7 +1540,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C25">
@@ -1581,7 +1581,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C26">
@@ -1622,7 +1622,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C27">
@@ -1663,7 +1663,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C28">
@@ -1704,7 +1704,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C29">
@@ -1745,7 +1745,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C30">
@@ -1786,7 +1786,7 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C31">
@@ -1827,7 +1827,7 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C32">
@@ -1868,7 +1868,7 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C33">
@@ -1909,7 +1909,7 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C34">
@@ -1950,7 +1950,7 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C35">
@@ -1991,7 +1991,7 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C36">
@@ -2055,9 +2055,9 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="e">
+      <c r="A2" t="str">
         <f>'Collected Minutiae'!Q2</f>
-        <v>#NUM!</v>
+        <v>464D520020323000000000F00000012C019000C500C5010000105B234047002F8F004073003CFA0080B6003D75008031005E94008087005D7E00805D006608004037007795008045008F0600402600A4A000405400A5910040C300A4E60040A100ACF20040B500B47100403900BD1D0040A700CBED0080DC00E9690080AB00DF7000409000E6F200405900DE9300404500E91A00402E0102AD00406600F00F00408C00ED800080B200F8E50080C5010DDB00408400FBF200409B010F6700802F013728004057011B190040A401455C00406B012CF700402B015E280080F70110620040D101736D0080C1018068000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>